<commit_message>
Conclusiones y documentación del proyecto.
</commit_message>
<xml_diff>
--- a/ResultadosComplejidad.xlsx
+++ b/ResultadosComplejidad.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\FCiencias\2022-1\IA\Otello\ProyectoOthello\GitOtello\Othello\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAB6C46-71FE-48CB-AE29-DBBEC612C5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E7CF933D-9D48-454C-AF32-3B471D17D187}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -64,12 +58,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,14 +103,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentual" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -132,25 +126,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-MX"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -600,7 +582,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E8E9-4952-8378-3FE40D21CE7F}"/>
             </c:ext>
@@ -1055,29 +1037,21 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-E8E9-4952-8378-3FE40D21CE7F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="567891048"/>
-        <c:axId val="567887440"/>
+        <c:dLbls/>
+        <c:axId val="209599104"/>
+        <c:axId val="209625472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="567891048"/>
+        <c:axId val="209599104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1096,7 +1070,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1124,16 +1097,15 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567887440"/>
+        <c:crossAx val="209625472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="567887440"/>
+        <c:axId val="209625472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1152,7 +1124,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1185,7 +1156,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567891048"/>
+        <c:crossAx val="209599104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1199,7 +1170,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1229,14 +1200,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1268,32 +1238,20 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-MX"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1359,8 +1317,6 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1759,7 +1715,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B4F5-4D54-B0CA-DF40941C1E75}"/>
             </c:ext>
@@ -1830,8 +1786,6 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -2230,7 +2184,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-B4F5-4D54-B0CA-DF40941C1E75}"/>
             </c:ext>
@@ -2301,8 +2255,6 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -2701,29 +2653,21 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-B4F5-4D54-B0CA-DF40941C1E75}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="567891048"/>
-        <c:axId val="567887440"/>
+        <c:dLbls/>
+        <c:axId val="211839232"/>
+        <c:axId val="211853312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="567891048"/>
+        <c:axId val="211839232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2742,7 +2686,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2775,16 +2718,15 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567887440"/>
+        <c:crossAx val="211853312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="567887440"/>
+        <c:axId val="211853312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2803,7 +2745,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2836,7 +2777,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567891048"/>
+        <c:crossAx val="211839232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2850,7 +2791,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2880,14 +2821,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2919,7 +2859,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4101,7 +4041,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E00ADF9-1D23-4FA1-BB5E-00ABABA55FF9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2E00ADF9-1D23-4FA1-BB5E-00ABABA55FF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4137,7 +4077,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4315CDE-67E2-42C4-A551-6655FA4761ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4315CDE-67E2-42C4-A551-6655FA4761ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4203,7 +4143,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4255,7 +4195,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4449,34 +4389,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4883F5A-D697-451D-8989-F7A2CE4429F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7265625" customWidth="1"/>
+    <col min="5" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" hidden="1" customWidth="1"/>
     <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4505,7 +4445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4548,7 +4488,7 @@
         <v>1712</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4591,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4634,7 +4574,7 @@
         <v>6345</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4677,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4720,7 +4660,7 @@
         <v>20697</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4763,7 +4703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4806,7 +4746,7 @@
         <v>17324</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4849,7 +4789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4892,7 +4832,7 @@
         <v>17126</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4935,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4978,7 +4918,7 @@
         <v>38744</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5021,7 +4961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5064,7 +5004,7 @@
         <v>20703</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5107,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5150,7 +5090,7 @@
         <v>29201</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5193,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5236,7 +5176,7 @@
         <v>27587</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5279,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5322,7 +5262,7 @@
         <v>25777</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5365,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5408,7 +5348,7 @@
         <v>58537</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5451,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5494,7 +5434,7 @@
         <v>89000</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5537,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5580,7 +5520,7 @@
         <v>101535</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5623,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5666,7 +5606,7 @@
         <v>72348</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5709,7 +5649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5752,7 +5692,7 @@
         <v>64931</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5795,7 +5735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5838,7 +5778,7 @@
         <v>150748</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5881,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5924,7 +5864,7 @@
         <v>123021</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5967,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6010,7 +5950,7 @@
         <v>156414</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6053,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6096,7 +6036,7 @@
         <v>80154</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6139,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6182,7 +6122,7 @@
         <v>37879</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6225,7 +6165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6268,7 +6208,7 @@
         <v>25229</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6311,7 +6251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6354,7 +6294,7 @@
         <v>8263</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6397,7 +6337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6440,7 +6380,7 @@
         <v>12790</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6483,7 +6423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6526,7 +6466,7 @@
         <v>10397</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6569,7 +6509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6612,7 +6552,7 @@
         <v>5528</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6655,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6698,7 +6638,7 @@
         <v>2532</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6741,7 +6681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6784,7 +6724,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6827,7 +6767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6870,7 +6810,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6913,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6956,7 +6896,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6999,7 +6939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60">
         <v>59</v>
       </c>
@@ -7042,7 +6982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61">
         <v>60</v>
       </c>
@@ -7085,7 +7025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62">
         <v>61</v>
       </c>
@@ -7128,7 +7068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63">
         <v>62</v>
       </c>
@@ -7171,7 +7111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64">
         <v>63</v>
       </c>
@@ -7213,7 +7153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:13">
       <c r="I65" s="3">
         <f>AVERAGE(I2:I64)</f>
         <v>0.4796546336684287</v>

</xml_diff>